<commit_message>
addition of html links
</commit_message>
<xml_diff>
--- a/input/html-links-ICTR.xlsx
+++ b/input/html-links-ICTR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\Nextcloud\IDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EFF9A9-CF50-4BFD-BEFB-5F41352FB92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194A0E67-4C06-4330-9C51-4A7576FBAFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26964" yWindow="4860" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="91">
   <si>
     <t>ICTR</t>
   </si>
@@ -88,16 +88,232 @@
   </si>
   <si>
     <t>ZF</t>
+  </si>
+  <si>
+    <t>CBI</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS12062R0000616281.DOC</t>
+  </si>
+  <si>
+    <t>ICTR-01-66-T</t>
+  </si>
+  <si>
+    <t>CDK / CBJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS18336R0000617492.DOC</t>
+  </si>
+  <si>
+    <t>CDL / CBR</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS12456R0000617514.DOC</t>
+  </si>
+  <si>
+    <t>CNJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS20656R0000617520.DOC</t>
+  </si>
+  <si>
+    <t>CBS</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS15607R0000616017.DOC</t>
+  </si>
+  <si>
+    <t>CBJ / CBN</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS16416R0000617500.DOC</t>
+  </si>
+  <si>
+    <t>YAU / YAT</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS13848R0000616022.DOC</t>
+  </si>
+  <si>
+    <t>CBS / CBT</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS16508R0000616014.DOC</t>
+  </si>
+  <si>
+    <t>accused</t>
+  </si>
+  <si>
+    <t>Seromba</t>
+  </si>
+  <si>
+    <t>GLM</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS20722R0000616773.DOC</t>
+  </si>
+  <si>
+    <t>ICTR-98-44-C-T</t>
+  </si>
+  <si>
+    <t>GII / GIT</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS17989R0000616779.DOC</t>
+  </si>
+  <si>
+    <t>AVD / GIN</t>
+  </si>
+  <si>
+    <t>GAC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS12873R0000616785.DOC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS15184R0000616793.DOC</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS12270R0000616799.DOC</t>
+  </si>
+  <si>
+    <t>GIO / ALW</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS15879R0000616816.DOC</t>
+  </si>
+  <si>
+    <t>ALW / XV</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS18774R0000616822.DOC</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS16926R0000616828.DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAREMERA et al. 	</t>
+  </si>
+  <si>
+    <t>Nzabonimana</t>
+  </si>
+  <si>
+    <t>AFB / UL</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS18018R0000627861.DOC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS15982R0000627908.DOC</t>
+  </si>
+  <si>
+    <t>ALG</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS14042R0000627928.DOC</t>
+  </si>
+  <si>
+    <t>KZ / BUO</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS20701R0000627932.DOC</t>
+  </si>
+  <si>
+    <t>BUO / DBN</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS14981R0000627936.DOC</t>
+  </si>
+  <si>
+    <t>ATQ / HAD</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS20793R0000630217.DOC</t>
+  </si>
+  <si>
+    <t>AWO</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS17093R0000628113.DOC</t>
+  </si>
+  <si>
+    <t>GLJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS19358R0000627926.DOC</t>
+  </si>
+  <si>
+    <t>RENZAHO</t>
+  </si>
+  <si>
+    <t>ICTR-97-31</t>
+  </si>
+  <si>
+    <t>TAK / TAC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS18956R0000615692.DOC</t>
+  </si>
+  <si>
+    <t>TBC / TAB</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS12464R0000628380.DOC</t>
+  </si>
+  <si>
+    <t>TBI / TBJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS15887R0000628527.DOC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS13707R0000615662.DOC</t>
+  </si>
+  <si>
+    <t>TAW</t>
+  </si>
+  <si>
+    <t>TAK / TAS / TBC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS16274R0000628379.DOC</t>
+  </si>
+  <si>
+    <t>TBJ / TBK</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS15390R0000615660.DOC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS13272R0000615697.DOC</t>
+  </si>
+  <si>
+    <t>GACUMBITSI</t>
+  </si>
+  <si>
+    <t>ICTR-01-64</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,20 +623,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="9.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="14.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -428,16 +648,19 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -445,16 +668,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>38077</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -462,16 +688,19 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>38092</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -479,16 +708,19 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>38104</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -496,16 +728,19 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>38111</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -513,16 +748,19 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>38635</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -530,16 +768,19 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>38770</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -547,16 +788,640 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>38855</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2">
+        <v>38264</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2">
+        <v>38271</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2">
+        <v>38372</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2">
+        <v>38377</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2">
+        <v>38265</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2">
+        <v>38275</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2">
+        <v>38259</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2">
+        <v>38266</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="2">
+        <v>38523</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2">
+        <v>38526</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2">
+        <v>38531</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="2">
+        <v>38537</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="2">
+        <v>38544</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="2">
+        <v>38589</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="2">
+        <v>38594</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="2">
+        <v>38597</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="2">
+        <v>39091</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="2">
+        <v>39093</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="2">
+        <v>39105</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="2">
+        <v>39107</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2">
+        <v>39111</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="2">
+        <v>39114</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="2">
+        <v>39120</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="2">
+        <v>39104</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="2">
+        <v>37837</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="2">
+        <v>37839</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="2">
+        <v>37851</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="2">
+        <v>37853</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="2">
+        <v>37777</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="2">
+        <v>37852</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="2">
+        <v>37854</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Addition of second batches of files
</commit_message>
<xml_diff>
--- a/input/html-links-ICTR.xlsx
+++ b/input/html-links-ICTR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\Nextcloud\IDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EFF9A9-CF50-4BFD-BEFB-5F41352FB92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194A0E67-4C06-4330-9C51-4A7576FBAFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26964" yWindow="4860" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="91">
   <si>
     <t>ICTR</t>
   </si>
@@ -88,16 +88,232 @@
   </si>
   <si>
     <t>ZF</t>
+  </si>
+  <si>
+    <t>CBI</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS12062R0000616281.DOC</t>
+  </si>
+  <si>
+    <t>ICTR-01-66-T</t>
+  </si>
+  <si>
+    <t>CDK / CBJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS18336R0000617492.DOC</t>
+  </si>
+  <si>
+    <t>CDL / CBR</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS12456R0000617514.DOC</t>
+  </si>
+  <si>
+    <t>CNJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS20656R0000617520.DOC</t>
+  </si>
+  <si>
+    <t>CBS</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS15607R0000616017.DOC</t>
+  </si>
+  <si>
+    <t>CBJ / CBN</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS16416R0000617500.DOC</t>
+  </si>
+  <si>
+    <t>YAU / YAT</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS13848R0000616022.DOC</t>
+  </si>
+  <si>
+    <t>CBS / CBT</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-66/TRS16508R0000616014.DOC</t>
+  </si>
+  <si>
+    <t>accused</t>
+  </si>
+  <si>
+    <t>Seromba</t>
+  </si>
+  <si>
+    <t>GLM</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS20722R0000616773.DOC</t>
+  </si>
+  <si>
+    <t>ICTR-98-44-C-T</t>
+  </si>
+  <si>
+    <t>GII / GIT</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS17989R0000616779.DOC</t>
+  </si>
+  <si>
+    <t>AVD / GIN</t>
+  </si>
+  <si>
+    <t>GAC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS12873R0000616785.DOC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS15184R0000616793.DOC</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS12270R0000616799.DOC</t>
+  </si>
+  <si>
+    <t>GIO / ALW</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS15879R0000616816.DOC</t>
+  </si>
+  <si>
+    <t>ALW / XV</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS18774R0000616822.DOC</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-98-44C/TRS16926R0000616828.DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAREMERA et al. 	</t>
+  </si>
+  <si>
+    <t>Nzabonimana</t>
+  </si>
+  <si>
+    <t>AFB / UL</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS18018R0000627861.DOC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS15982R0000627908.DOC</t>
+  </si>
+  <si>
+    <t>ALG</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS14042R0000627928.DOC</t>
+  </si>
+  <si>
+    <t>KZ / BUO</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS20701R0000627932.DOC</t>
+  </si>
+  <si>
+    <t>BUO / DBN</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS14981R0000627936.DOC</t>
+  </si>
+  <si>
+    <t>ATQ / HAD</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS20793R0000630217.DOC</t>
+  </si>
+  <si>
+    <t>AWO</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS17093R0000628113.DOC</t>
+  </si>
+  <si>
+    <t>GLJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-97-31/TRS19358R0000627926.DOC</t>
+  </si>
+  <si>
+    <t>RENZAHO</t>
+  </si>
+  <si>
+    <t>ICTR-97-31</t>
+  </si>
+  <si>
+    <t>TAK / TAC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS18956R0000615692.DOC</t>
+  </si>
+  <si>
+    <t>TBC / TAB</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS12464R0000628380.DOC</t>
+  </si>
+  <si>
+    <t>TBI / TBJ</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS15887R0000628527.DOC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS13707R0000615662.DOC</t>
+  </si>
+  <si>
+    <t>TAW</t>
+  </si>
+  <si>
+    <t>TAK / TAS / TBC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS16274R0000628379.DOC</t>
+  </si>
+  <si>
+    <t>TBJ / TBK</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS15390R0000615660.DOC</t>
+  </si>
+  <si>
+    <t>https://ucr.irmct.org/LegalRef/CMSDocStore/Public/English/Transcript/NotIndexable/ICTR-01-64/TRS13272R0000615697.DOC</t>
+  </si>
+  <si>
+    <t>GACUMBITSI</t>
+  </si>
+  <si>
+    <t>ICTR-01-64</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,20 +623,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="9.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="14.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -428,16 +648,19 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -445,16 +668,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>38077</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -462,16 +688,19 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>38092</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -479,16 +708,19 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>38104</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -496,16 +728,19 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>38111</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -513,16 +748,19 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>38635</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -530,16 +768,19 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>38770</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -547,16 +788,640 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>38855</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2">
+        <v>38264</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2">
+        <v>38271</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2">
+        <v>38372</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2">
+        <v>38377</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2">
+        <v>38265</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2">
+        <v>38275</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2">
+        <v>38259</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2">
+        <v>38266</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="2">
+        <v>38523</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2">
+        <v>38526</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2">
+        <v>38531</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="2">
+        <v>38537</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="2">
+        <v>38544</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="2">
+        <v>38589</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="2">
+        <v>38594</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="2">
+        <v>38597</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="2">
+        <v>39091</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="2">
+        <v>39093</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="2">
+        <v>39105</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="2">
+        <v>39107</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2">
+        <v>39111</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="2">
+        <v>39114</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="2">
+        <v>39120</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="2">
+        <v>39104</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="2">
+        <v>37837</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="2">
+        <v>37839</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="2">
+        <v>37851</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="2">
+        <v>37853</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="2">
+        <v>37777</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="2">
+        <v>37852</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="2">
+        <v>37854</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>